<commit_message>
draft with edit functionality
</commit_message>
<xml_diff>
--- a/personal_finance.xlsx
+++ b/personal_finance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.losi\_personal\Coding\personal_finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DECBF0-CA1C-4657-83C9-8E8B58C71F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F598F-AAA5-4A41-B917-AD5AD44B403B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" activeTab="3" xr2:uid="{757DA688-7504-40EC-BBE6-04C68CEC2EAD}"/>
   </bookViews>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -272,6 +272,69 @@
   </si>
   <si>
     <t>fine</t>
+  </si>
+  <si>
+    <t>amazon refund</t>
+  </si>
+  <si>
+    <t>bank refund</t>
+  </si>
+  <si>
+    <t>bank taxes</t>
+  </si>
+  <si>
+    <t>hotel istanbul airport</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>food out</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>clothes</t>
+  </si>
+  <si>
+    <t>gelato</t>
+  </si>
+  <si>
+    <t>gas bill</t>
+  </si>
+  <si>
+    <t>house shopping</t>
+  </si>
+  <si>
+    <t>iliad</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>money change</t>
+  </si>
+  <si>
+    <t>ATM withdrawal</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>dinner out</t>
+  </si>
+  <si>
+    <t>bike tyres</t>
+  </si>
+  <si>
+    <t>visa - cash withdraw chad</t>
+  </si>
+  <si>
+    <t>out + flights</t>
+  </si>
+  <si>
+    <t>coffee</t>
   </si>
 </sst>
 </file>
@@ -358,8 +421,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}" name="incomes" displayName="incomes" ref="A1:F69" totalsRowShown="0">
-  <autoFilter ref="A1:F69" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}" name="incomes" displayName="incomes" ref="A1:F75" totalsRowShown="0">
+  <autoFilter ref="A1:F75" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}">
+    <filterColumn colId="0">
+      <filters calendarType="gregorian">
+        <dateGroupItem year="2024" month="4" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
     <sortCondition ref="A1:A66"/>
   </sortState>
@@ -378,8 +447,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99C7F050-ADBC-42EF-BC97-BA312E69053C}" name="expenses" displayName="expenses" ref="A1:F97" totalsRowShown="0">
-  <autoFilter ref="A1:F97" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99C7F050-ADBC-42EF-BC97-BA312E69053C}" name="expenses" displayName="expenses" ref="A1:F134" totalsRowShown="0">
+  <autoFilter ref="A1:F134" xr:uid="{FE5F6759-440A-4F24-8BDE-4C7C878A4959}">
+    <filterColumn colId="0">
+      <filters calendarType="gregorian">
+        <dateGroupItem year="2024" month="4" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="revolut_EUR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F82">
     <sortCondition ref="A1:A82"/>
   </sortState>
@@ -835,10 +915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44752AA-0EEF-4BAF-A1AE-BF74CE7F9AF6}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -871,7 +951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43799</v>
       </c>
@@ -892,7 +972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43830</v>
       </c>
@@ -913,7 +993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43861</v>
       </c>
@@ -934,7 +1014,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43889</v>
       </c>
@@ -955,7 +1035,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43921</v>
       </c>
@@ -976,7 +1056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43951</v>
       </c>
@@ -997,7 +1077,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43982</v>
       </c>
@@ -1018,7 +1098,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44012</v>
       </c>
@@ -1039,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44043</v>
       </c>
@@ -1060,7 +1140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44074</v>
       </c>
@@ -1081,7 +1161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44104</v>
       </c>
@@ -1102,7 +1182,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44135</v>
       </c>
@@ -1123,7 +1203,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44165</v>
       </c>
@@ -1144,7 +1224,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44196</v>
       </c>
@@ -1165,7 +1245,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44196</v>
       </c>
@@ -1186,7 +1266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44196</v>
       </c>
@@ -1207,7 +1287,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44227</v>
       </c>
@@ -1228,7 +1308,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44255</v>
       </c>
@@ -1249,7 +1329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44286</v>
       </c>
@@ -1270,7 +1350,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44316</v>
       </c>
@@ -1291,7 +1371,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44347</v>
       </c>
@@ -1312,7 +1392,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44377</v>
       </c>
@@ -1333,7 +1413,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44408</v>
       </c>
@@ -1354,7 +1434,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44439</v>
       </c>
@@ -1375,7 +1455,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44469</v>
       </c>
@@ -1396,7 +1476,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44500</v>
       </c>
@@ -1417,7 +1497,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44530</v>
       </c>
@@ -1438,7 +1518,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44561</v>
       </c>
@@ -1459,7 +1539,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44561</v>
       </c>
@@ -1480,7 +1560,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44561</v>
       </c>
@@ -1501,7 +1581,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44592</v>
       </c>
@@ -1522,7 +1602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44620</v>
       </c>
@@ -1543,7 +1623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44651</v>
       </c>
@@ -1564,7 +1644,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44681</v>
       </c>
@@ -1585,7 +1665,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44712</v>
       </c>
@@ -1606,7 +1686,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44742</v>
       </c>
@@ -1627,7 +1707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44773</v>
       </c>
@@ -1648,7 +1728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44804</v>
       </c>
@@ -1669,7 +1749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44834</v>
       </c>
@@ -1690,7 +1770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44865</v>
       </c>
@@ -1711,7 +1791,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44895</v>
       </c>
@@ -1732,7 +1812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44926</v>
       </c>
@@ -1753,7 +1833,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44926</v>
       </c>
@@ -1774,7 +1854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44926</v>
       </c>
@@ -1795,7 +1875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44957</v>
       </c>
@@ -1816,7 +1896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44985</v>
       </c>
@@ -1837,7 +1917,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>45016</v>
       </c>
@@ -1858,7 +1938,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>45046</v>
       </c>
@@ -1879,7 +1959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>45077</v>
       </c>
@@ -1900,7 +1980,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>45107</v>
       </c>
@@ -1921,7 +2001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>45138</v>
       </c>
@@ -1942,7 +2022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>45169</v>
       </c>
@@ -1963,7 +2043,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>45199</v>
       </c>
@@ -1984,7 +2064,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>45230</v>
       </c>
@@ -2005,7 +2085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>45260</v>
       </c>
@@ -2026,7 +2106,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>45260</v>
       </c>
@@ -2047,7 +2127,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>45291</v>
       </c>
@@ -2068,7 +2148,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>45322</v>
       </c>
@@ -2089,7 +2169,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>45322</v>
       </c>
@@ -2110,7 +2190,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>45351</v>
       </c>
@@ -2131,7 +2211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>45351</v>
       </c>
@@ -2152,7 +2232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>45363</v>
       </c>
@@ -2173,7 +2253,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>45365</v>
       </c>
@@ -2194,7 +2274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>45365</v>
       </c>
@@ -2215,7 +2295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>45366</v>
       </c>
@@ -2236,7 +2316,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>45378</v>
       </c>
@@ -2296,6 +2376,132 @@
         <v>1212</v>
       </c>
       <c r="F69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>45398</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E70" s="1">
+        <v>59.18</v>
+      </c>
+      <c r="F70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>45404</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E71" s="1">
+        <v>12.17</v>
+      </c>
+      <c r="F71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>45408</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E72" s="1">
+        <v>5388.15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>45410</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E73" s="1">
+        <v>5.03</v>
+      </c>
+      <c r="F73" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>45411</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E74" s="1">
+        <v>500</v>
+      </c>
+      <c r="F74" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" t="str">
+        <f>INDEX(accounts[currency],MATCH(incomes[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1312</v>
+      </c>
+      <c r="F75" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2312,7 +2518,7 @@
           <x14:formula1>
             <xm:f>accounts!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B69</xm:sqref>
+          <xm:sqref>B2:B75</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2322,17 +2528,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41E4E0E-3D8F-4663-BE3B-C5FF4609020C}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
@@ -2359,7 +2565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43830</v>
       </c>
@@ -2381,7 +2587,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43830</v>
       </c>
@@ -2402,7 +2608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43861</v>
       </c>
@@ -2423,7 +2629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43951</v>
       </c>
@@ -2444,7 +2650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44012</v>
       </c>
@@ -2465,7 +2671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44043</v>
       </c>
@@ -2486,7 +2692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44074</v>
       </c>
@@ -2507,7 +2713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44074</v>
       </c>
@@ -2528,7 +2734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44104</v>
       </c>
@@ -2549,7 +2755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44135</v>
       </c>
@@ -2570,7 +2776,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44165</v>
       </c>
@@ -2591,7 +2797,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44196</v>
       </c>
@@ -2612,7 +2818,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44196</v>
       </c>
@@ -2633,7 +2839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44227</v>
       </c>
@@ -2654,7 +2860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44227</v>
       </c>
@@ -2675,7 +2881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44255</v>
       </c>
@@ -2696,7 +2902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44316</v>
       </c>
@@ -2717,7 +2923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44347</v>
       </c>
@@ -2738,7 +2944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44347</v>
       </c>
@@ -2759,7 +2965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44377</v>
       </c>
@@ -2780,7 +2986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44408</v>
       </c>
@@ -2801,7 +3007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44439</v>
       </c>
@@ -2822,7 +3028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44500</v>
       </c>
@@ -2843,7 +3049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44530</v>
       </c>
@@ -2864,7 +3070,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44561</v>
       </c>
@@ -2885,7 +3091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44561</v>
       </c>
@@ -2906,7 +3112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44561</v>
       </c>
@@ -2927,7 +3133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44592</v>
       </c>
@@ -2948,7 +3154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44592</v>
       </c>
@@ -2969,7 +3175,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44620</v>
       </c>
@@ -2990,7 +3196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44651</v>
       </c>
@@ -3011,7 +3217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44681</v>
       </c>
@@ -3032,7 +3238,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44712</v>
       </c>
@@ -3053,7 +3259,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44742</v>
       </c>
@@ -3074,7 +3280,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44773</v>
       </c>
@@ -3095,7 +3301,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44804</v>
       </c>
@@ -3116,7 +3322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44834</v>
       </c>
@@ -3137,7 +3343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44865</v>
       </c>
@@ -3158,7 +3364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44895</v>
       </c>
@@ -3179,7 +3385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44926</v>
       </c>
@@ -3200,7 +3406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44926</v>
       </c>
@@ -3221,7 +3427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44926</v>
       </c>
@@ -3242,7 +3448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44926</v>
       </c>
@@ -3263,7 +3469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44957</v>
       </c>
@@ -3284,7 +3490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44985</v>
       </c>
@@ -3305,7 +3511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45016</v>
       </c>
@@ -3326,7 +3532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>45046</v>
       </c>
@@ -3347,7 +3553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>45046</v>
       </c>
@@ -3368,7 +3574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>45077</v>
       </c>
@@ -3389,7 +3595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>45107</v>
       </c>
@@ -3410,7 +3616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>45107</v>
       </c>
@@ -3431,7 +3637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>45138</v>
       </c>
@@ -3452,7 +3658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>45138</v>
       </c>
@@ -3473,7 +3679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>45169</v>
       </c>
@@ -3494,7 +3700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>45169</v>
       </c>
@@ -3515,7 +3721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>45199</v>
       </c>
@@ -3536,7 +3742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>45199</v>
       </c>
@@ -3557,7 +3763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>45230</v>
       </c>
@@ -3578,7 +3784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>45260</v>
       </c>
@@ -3599,7 +3805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>45260</v>
       </c>
@@ -3620,7 +3826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>45260</v>
       </c>
@@ -3641,7 +3847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>45291</v>
       </c>
@@ -3662,7 +3868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>45291</v>
       </c>
@@ -3683,7 +3889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>45322</v>
       </c>
@@ -3704,7 +3910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>45322</v>
       </c>
@@ -3725,7 +3931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>45322</v>
       </c>
@@ -3746,7 +3952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>45351</v>
       </c>
@@ -3767,7 +3973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>45351</v>
       </c>
@@ -3788,7 +3994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>45351</v>
       </c>
@@ -3809,7 +4015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>45351</v>
       </c>
@@ -3830,7 +4036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>45359</v>
       </c>
@@ -3851,7 +4057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>45365</v>
       </c>
@@ -3872,7 +4078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>45365</v>
       </c>
@@ -3893,7 +4099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>45366</v>
       </c>
@@ -3914,7 +4120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>45366</v>
       </c>
@@ -3936,7 +4142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>45368</v>
       </c>
@@ -3957,7 +4163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>45369</v>
       </c>
@@ -3978,7 +4184,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>45369</v>
       </c>
@@ -3999,7 +4205,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>45370</v>
       </c>
@@ -4021,7 +4227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>45371</v>
       </c>
@@ -4042,7 +4248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>45372</v>
       </c>
@@ -4063,7 +4269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>45372</v>
       </c>
@@ -4084,7 +4290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>45373</v>
       </c>
@@ -4105,7 +4311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>45378</v>
       </c>
@@ -4126,7 +4332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>45378</v>
       </c>
@@ -4147,7 +4353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>45373</v>
       </c>
@@ -4169,7 +4375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>45375</v>
       </c>
@@ -4191,7 +4397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>45379</v>
       </c>
@@ -4213,7 +4419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>45380</v>
       </c>
@@ -4234,7 +4440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>45382</v>
       </c>
@@ -4256,7 +4462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>45383</v>
       </c>
@@ -4277,7 +4483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>45380</v>
       </c>
@@ -4298,7 +4504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>45384</v>
       </c>
@@ -4319,7 +4525,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>45383</v>
       </c>
@@ -4340,7 +4546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>45384</v>
       </c>
@@ -4361,7 +4567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>45385</v>
       </c>
@@ -4379,6 +4585,785 @@
         <v>307.13</v>
       </c>
       <c r="F97" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>45387</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E98" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="F98" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>45389</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>23</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E99" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="F99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>45391</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>57</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E100" s="1">
+        <v>280</v>
+      </c>
+      <c r="F100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>58</v>
+      </c>
+      <c r="D101" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E101" s="1">
+        <v>92.1</v>
+      </c>
+      <c r="F101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>45409</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" t="s">
+        <v>59</v>
+      </c>
+      <c r="D102" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E102" s="1">
+        <f>24.27+5.99+15.57</f>
+        <v>45.83</v>
+      </c>
+      <c r="F102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>45410</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" t="s">
+        <v>60</v>
+      </c>
+      <c r="D103" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E103" s="1">
+        <v>25</v>
+      </c>
+      <c r="F103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>45410</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>61</v>
+      </c>
+      <c r="D104" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E104" s="1">
+        <v>33.97</v>
+      </c>
+      <c r="F104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>45410</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>62</v>
+      </c>
+      <c r="D105" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E105" s="1">
+        <v>5</v>
+      </c>
+      <c r="F105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>45411</v>
+      </c>
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>63</v>
+      </c>
+      <c r="D106" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E106" s="1">
+        <v>200</v>
+      </c>
+      <c r="F106" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>45411</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>64</v>
+      </c>
+      <c r="D107" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E107" s="1">
+        <v>3</v>
+      </c>
+      <c r="F107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>45385</v>
+      </c>
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E108" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="F108" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>45386</v>
+      </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>34</v>
+      </c>
+      <c r="D109" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E109" s="1">
+        <v>50.56</v>
+      </c>
+      <c r="F109" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>45387</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>65</v>
+      </c>
+      <c r="D110" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E110" s="1">
+        <v>15</v>
+      </c>
+      <c r="F110" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>45387</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E111" s="1">
+        <v>49.2</v>
+      </c>
+      <c r="F111" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>45388</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>34</v>
+      </c>
+      <c r="D112" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E112" s="1">
+        <v>21.13</v>
+      </c>
+      <c r="F112" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>45389</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>34</v>
+      </c>
+      <c r="D113" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E113" s="1">
+        <v>40.89</v>
+      </c>
+      <c r="F113" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>45390</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>66</v>
+      </c>
+      <c r="D114" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E114" s="1">
+        <v>112.31</v>
+      </c>
+      <c r="F114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>45391</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>59</v>
+      </c>
+      <c r="D115" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E115" s="1">
+        <v>43.18</v>
+      </c>
+      <c r="F115" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>45392</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>67</v>
+      </c>
+      <c r="D116" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E116" s="1">
+        <v>50</v>
+      </c>
+      <c r="F116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>45394</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>68</v>
+      </c>
+      <c r="D117" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E117" s="1">
+        <v>94.01</v>
+      </c>
+      <c r="F117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>45411</v>
+      </c>
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" t="s">
+        <v>52</v>
+      </c>
+      <c r="D118" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E118" s="1">
+        <v>500</v>
+      </c>
+      <c r="F118" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>69</v>
+      </c>
+      <c r="D119" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E119" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="F119" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E120" s="1">
+        <v>2424</v>
+      </c>
+      <c r="F120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>70</v>
+      </c>
+      <c r="D121" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E121" s="1">
+        <v>31</v>
+      </c>
+      <c r="F121" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>45415</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>71</v>
+      </c>
+      <c r="D122" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E122" s="1">
+        <v>350</v>
+      </c>
+      <c r="F122" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>45415</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E123" s="1">
+        <v>10</v>
+      </c>
+      <c r="F123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B124" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" t="s">
+        <v>72</v>
+      </c>
+      <c r="D124" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E124" s="1">
+        <v>53.18</v>
+      </c>
+      <c r="F124" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" t="s">
+        <v>36</v>
+      </c>
+      <c r="D125" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E125" s="1">
+        <v>211.85</v>
+      </c>
+      <c r="F125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>45416</v>
+      </c>
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>73</v>
+      </c>
+      <c r="D126" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E126" s="1">
+        <v>287.42</v>
+      </c>
+      <c r="F126" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>45417</v>
+      </c>
+      <c r="B127" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E127" s="1">
+        <v>34.35</v>
+      </c>
+      <c r="F127" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>45418</v>
+      </c>
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s">
+        <v>34</v>
+      </c>
+      <c r="D128" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E128" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="F128" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
+        <v>74</v>
+      </c>
+      <c r="D129" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E129" s="1">
+        <v>4</v>
+      </c>
+      <c r="F129" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E130" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="F130" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B131" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" t="s">
+        <v>34</v>
+      </c>
+      <c r="D131" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E131" s="1">
+        <f>33.72+11.27+9.61</f>
+        <v>54.599999999999994</v>
+      </c>
+      <c r="F131" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>45423</v>
+      </c>
+      <c r="B132" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E132" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="F132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>45424</v>
+      </c>
+      <c r="B133" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E133" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="F133" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>45426</v>
+      </c>
+      <c r="B134" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" t="s">
+        <v>34</v>
+      </c>
+      <c r="D134" t="str">
+        <f>INDEX(accounts[currency],MATCH(expenses[[#This Row],[account]],accounts[name],0))</f>
+        <v>EUR</v>
+      </c>
+      <c r="E134" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="F134" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4395,7 +5380,7 @@
           <x14:formula1>
             <xm:f>accounts!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B97</xm:sqref>
+          <xm:sqref>B2:B134</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4405,10 +5390,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DC3777-5361-4D69-A5C8-6CED5BAC1CEC}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -4468,7 +5453,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C25" si="0">B4+C3</f>
+        <f t="shared" ref="C4:C26" si="0">B4+C3</f>
         <v>7000</v>
       </c>
       <c r="D4">
@@ -4788,6 +5773,35 @@
       </c>
       <c r="D25">
         <v>63440.76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>53400</v>
+      </c>
+      <c r="D26">
+        <v>61715.54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>53400</v>
+      </c>
+      <c r="D27">
+        <v>63316.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>